<commit_message>
Update and uniform 256,512 and all nRsnn ready
</commit_message>
<xml_diff>
--- a/SHDFinal/RecurrentSNN/Training-TestAccuracies.xlsx
+++ b/SHDFinal/RecurrentSNN/Training-TestAccuracies.xlsx
@@ -450,7 +450,7 @@
   <dimension ref="D4:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,12 +619,24 @@
       <c r="F9" s="4">
         <v>0.58299999999999996</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4"/>
+      <c r="G9" s="3">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.878</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.63100000000000001</v>
+      </c>
       <c r="M9" s="3">
         <v>0.91</v>
       </c>

</xml_diff>